<commit_message>
Major and Minor Groups
Basically have owl's for Major and Minor Groups
</commit_message>
<xml_diff>
--- a/src/ontology/Ontorat input files/Ax_SOC Major Groups V011.xlsx
+++ b/src/ontology/Ontorat input files/Ax_SOC Major Groups V011.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samal\Documents\GitHub\OccO_Dev\src\ontology\Ontorat input files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9DFA4A-ABC9-41F6-92DB-E485FE16296C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2327CE7E-0A23-4900-97B0-6A7CD0B492D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="1890" windowWidth="23850" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="2235" windowWidth="23850" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOC-MajorGroups" sheetId="1" r:id="rId1"/>
@@ -9152,34 +9152,34 @@
     <t>OccO_55000000</t>
   </si>
   <si>
+    <t>Column Headings (Guideline is that BOLD headings [*] are input to Ontorat)</t>
+  </si>
+  <si>
+    <t>8-digit suffix</t>
+  </si>
+  <si>
+    <t>Two additional digits were required for new O*Net additional occupations for new fields of work</t>
+  </si>
+  <si>
+    <t>OccO ID derived from SOC as two-digin major group + 4 digit SOC Detailed Occup. + 2  digit O*Net</t>
+  </si>
+  <si>
+    <t>Preparing for inclusion in Github project documentation plus input data</t>
+  </si>
+  <si>
+    <t>filename:  Ax_SOC Major Groups V011.xlsx</t>
+  </si>
+  <si>
+    <t>Version V0.1.1</t>
+  </si>
+  <si>
+    <t>OccO OntoRat Input File: Level A - Major Groups</t>
+  </si>
+  <si>
+    <t>O*Net -SOC Id</t>
+  </si>
+  <si>
     <t>OccO_00000001</t>
-  </si>
-  <si>
-    <t>Column Headings (Guideline is that BOLD headings [*] are input to Ontorat)</t>
-  </si>
-  <si>
-    <t>8-digit suffix</t>
-  </si>
-  <si>
-    <t>Two additional digits were required for new O*Net additional occupations for new fields of work</t>
-  </si>
-  <si>
-    <t>OccO ID derived from SOC as two-digin major group + 4 digit SOC Detailed Occup. + 2  digit O*Net</t>
-  </si>
-  <si>
-    <t>Preparing for inclusion in Github project documentation plus input data</t>
-  </si>
-  <si>
-    <t>filename:  Ax_SOC Major Groups V011.xlsx</t>
-  </si>
-  <si>
-    <t>Version V0.1.1</t>
-  </si>
-  <si>
-    <t>OccO OntoRat Input File: Level A - Major Groups</t>
-  </si>
-  <si>
-    <t>O*Net -SOC Id</t>
   </si>
 </sst>
 </file>
@@ -9718,14 +9718,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -10108,14 +10108,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="1" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="56.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.5703125" customWidth="1"/>
@@ -10131,7 +10130,7 @@
         <v>67</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3047</v>
+        <v>3046</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>55</v>
@@ -10154,7 +10153,7 @@
         <v>3015</v>
       </c>
       <c r="B2" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -10180,7 +10179,7 @@
         <v>3016</v>
       </c>
       <c r="B3" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -10206,7 +10205,7 @@
         <v>3017</v>
       </c>
       <c r="B4" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -10232,7 +10231,7 @@
         <v>3018</v>
       </c>
       <c r="B5" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -10258,7 +10257,7 @@
         <v>3019</v>
       </c>
       <c r="B6" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -10284,7 +10283,7 @@
         <v>3020</v>
       </c>
       <c r="B7" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -10310,7 +10309,7 @@
         <v>3021</v>
       </c>
       <c r="B8" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -10336,7 +10335,7 @@
         <v>3022</v>
       </c>
       <c r="B9" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -10362,7 +10361,7 @@
         <v>3023</v>
       </c>
       <c r="B10" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -10388,7 +10387,7 @@
         <v>3024</v>
       </c>
       <c r="B11" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -10414,7 +10413,7 @@
         <v>3025</v>
       </c>
       <c r="B12" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -10440,7 +10439,7 @@
         <v>3026</v>
       </c>
       <c r="B13" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -10466,7 +10465,7 @@
         <v>3027</v>
       </c>
       <c r="B14" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -10492,7 +10491,7 @@
         <v>3028</v>
       </c>
       <c r="B15" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -10518,7 +10517,7 @@
         <v>3029</v>
       </c>
       <c r="B16" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -10544,7 +10543,7 @@
         <v>3030</v>
       </c>
       <c r="B17" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -10570,7 +10569,7 @@
         <v>3031</v>
       </c>
       <c r="B18" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -10596,7 +10595,7 @@
         <v>3032</v>
       </c>
       <c r="B19" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -10622,7 +10621,7 @@
         <v>3033</v>
       </c>
       <c r="B20" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -10648,7 +10647,7 @@
         <v>3034</v>
       </c>
       <c r="B21" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
@@ -10674,7 +10673,7 @@
         <v>3035</v>
       </c>
       <c r="B22" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -10700,7 +10699,7 @@
         <v>3036</v>
       </c>
       <c r="B23" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -10726,7 +10725,7 @@
         <v>3037</v>
       </c>
       <c r="B24" t="s">
-        <v>3038</v>
+        <v>3047</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
@@ -10757,7 +10756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4659D1-E66A-4FF8-BF6B-C3168C62A716}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -10771,17 +10770,17 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1" s="3" t="s">
-        <v>3046</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
+        <v>3043</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
         <v>3044</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="11" t="s">
-        <v>3045</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -10847,12 +10846,12 @@
         <v>44607</v>
       </c>
       <c r="C14" t="s">
-        <v>3043</v>
+        <v>3042</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>3039</v>
+        <v>3038</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -10863,7 +10862,7 @@
         <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>3042</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -10924,10 +10923,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>3039</v>
+      </c>
+      <c r="C25" t="s">
         <v>3040</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3041</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -10969,24 +10968,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">

</xml_diff>